<commit_message>
Changes made in the Transactions file in ceating the Layering chains. And updated the Data Dictionary file.
</commit_message>
<xml_diff>
--- a/Data Dictionary.xlsx
+++ b/Data Dictionary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fc4bd521ffc22738/Desktop/Freelancing/AIGEN/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fc4bd521ffc22738/Desktop/Freelancing/AIGEN/smartsentry_aml_model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E8E6087-2FD7-42AA-9DC6-118DBB4092B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{4E8E6087-2FD7-42AA-9DC6-118DBB4092B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{055F9C7F-6D0C-48D7-AD23-F4A5C58C2F29}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer &amp; Account" sheetId="1" r:id="rId1"/>
@@ -540,32 +540,6 @@
 • Multiple accounts use the same device.
 • All accounts funnel funds to a single high-risk exit beneficiary.
 • Each account performs multiple transactions.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Pattern:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> A → B → C → D
-Graph Shape: ➝ Linear chain
-• Funds hop across 3–4 internal accounts.
-• Transfers occur within minutes.</t>
     </r>
   </si>
   <si>
@@ -742,6 +716,32 @@
   </si>
   <si>
     <t>Not useful if it is just debit and wrt to sender side</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pattern:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> A → B → C → A
+Graph Shape: ➝ Linear chain
+• Funds hop across 3–4 internal accounts.
+• Transfers occur within minutes.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -882,7 +882,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -894,12 +894,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -907,9 +901,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -944,10 +935,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1301,7 +1295,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:E35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
@@ -1311,16 +1305,16 @@
     <col min="2" max="2" width="23.5546875" style="4" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.44140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="124.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="124.5546875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
@@ -1332,21 +1326,21 @@
       <c r="D3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="9" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1360,7 +1354,7 @@
       <c r="D5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1374,7 +1368,7 @@
       <c r="D6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="7" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1388,7 +1382,7 @@
       <c r="D7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="7" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1402,7 +1396,7 @@
       <c r="D8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="7" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1416,7 +1410,7 @@
       <c r="D9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1430,7 +1424,7 @@
       <c r="D10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="7" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1444,7 +1438,7 @@
       <c r="D11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="7" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1458,7 +1452,7 @@
       <c r="D12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="7" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1472,7 +1466,7 @@
       <c r="D13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="7" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1486,49 +1480,43 @@
       <c r="D14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="10"/>
-    </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="D17" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E17" s="22" t="s">
+      <c r="E17" s="19" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E18" s="9" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1542,7 +1530,7 @@
       <c r="D19" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="7" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1556,49 +1544,43 @@
       <c r="D20" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="10"/>
-    </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="21" t="s">
+      <c r="C23" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D23" s="21" t="s">
+      <c r="D23" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E23" s="22" t="s">
+      <c r="E23" s="19" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D24" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="E24" s="9" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1612,7 +1594,7 @@
       <c r="D25" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="E25" s="7" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1626,7 +1608,7 @@
       <c r="D26" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="9" t="s">
+      <c r="E26" s="7" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1640,7 +1622,7 @@
       <c r="D27" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E27" s="9" t="s">
+      <c r="E27" s="7" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1654,7 +1636,7 @@
       <c r="D28" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E28" s="9" t="s">
+      <c r="E28" s="7" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1668,49 +1650,43 @@
       <c r="D29" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="9" t="s">
+      <c r="E29" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="10"/>
-    </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B31" s="23" t="s">
+      <c r="B31" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B32" s="21" t="s">
+      <c r="B32" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C32" s="21" t="s">
+      <c r="C32" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D32" s="21" t="s">
+      <c r="D32" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E32" s="22" t="s">
+      <c r="E32" s="19" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D33" s="11" t="s">
+      <c r="D33" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E33" s="12" t="s">
+      <c r="E33" s="9" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1724,7 +1700,7 @@
       <c r="D34" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E34" s="9" t="s">
+      <c r="E34" s="7" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1738,7 +1714,7 @@
       <c r="D35" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E35" s="9" t="s">
+      <c r="E35" s="7" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1779,93 +1755,93 @@
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="D2" s="11" t="s">
+      <c r="C2" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="18" t="s">
-        <v>188</v>
-      </c>
-      <c r="D3" s="18" t="s">
+      <c r="C3" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="C4" s="18" t="s">
-        <v>188</v>
-      </c>
-      <c r="D4" s="18" t="s">
+      <c r="C4" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="D4" s="15" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>188</v>
-      </c>
-      <c r="D5" s="18" t="s">
+      <c r="C5" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="D5" s="15" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="C6" s="18" t="s">
-        <v>188</v>
-      </c>
-      <c r="D6" s="18" t="s">
+      <c r="C6" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="D6" s="15" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>188</v>
-      </c>
-      <c r="D7" s="18" t="s">
+      <c r="C7" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="D7" s="15" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1877,7 +1853,7 @@
         <v>98</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>99</v>
@@ -1891,7 +1867,7 @@
         <v>101</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>99</v>
@@ -1905,7 +1881,7 @@
         <v>103</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>99</v>
@@ -1919,13 +1895,13 @@
         <v>105</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E11" s="24" t="s">
-        <v>189</v>
+      <c r="E11" s="20" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -1936,7 +1912,7 @@
         <v>107</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>99</v>
@@ -1950,7 +1926,7 @@
         <v>109</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>99</v>
@@ -1964,7 +1940,7 @@
         <v>111</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>99</v>
@@ -1978,7 +1954,7 @@
         <v>113</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>99</v>
@@ -1989,10 +1965,10 @@
         <v>34</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>99</v>
@@ -2003,10 +1979,10 @@
         <v>37</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>99</v>
@@ -2017,10 +1993,10 @@
         <v>23</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>99</v>
@@ -2031,10 +2007,10 @@
         <v>27</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>99</v>
@@ -2045,10 +2021,10 @@
         <v>25</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>99</v>
@@ -2059,10 +2035,10 @@
         <v>11</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>99</v>
@@ -2073,10 +2049,10 @@
         <v>14</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>99</v>
@@ -2087,10 +2063,10 @@
         <v>17</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>99</v>
@@ -2101,10 +2077,10 @@
         <v>19</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>99</v>
@@ -2115,10 +2091,10 @@
         <v>21</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>99</v>
@@ -2129,10 +2105,10 @@
         <v>42</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>99</v>
@@ -2143,10 +2119,10 @@
         <v>44</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>99</v>
@@ -2157,10 +2133,10 @@
         <v>46</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>99</v>
@@ -2171,10 +2147,10 @@
         <v>48</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>99</v>
@@ -2185,10 +2161,10 @@
         <v>50</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>99</v>
@@ -2199,10 +2175,10 @@
         <v>55</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>99</v>
@@ -2213,10 +2189,10 @@
         <v>57</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>99</v>
@@ -2230,7 +2206,7 @@
         <v>115</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>99</v>
@@ -2244,7 +2220,7 @@
         <v>117</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>99</v>
@@ -2258,7 +2234,7 @@
         <v>119</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>99</v>
@@ -2272,7 +2248,7 @@
         <v>121</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>99</v>
@@ -2286,7 +2262,7 @@
         <v>123</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>99</v>
@@ -2300,7 +2276,7 @@
         <v>125</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>99</v>
@@ -2314,7 +2290,7 @@
         <v>127</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>99</v>
@@ -2328,7 +2304,7 @@
         <v>129</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>99</v>
@@ -2342,7 +2318,7 @@
         <v>131</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>99</v>
@@ -2356,7 +2332,7 @@
         <v>133</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>99</v>
@@ -2370,7 +2346,7 @@
         <v>135</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>99</v>
@@ -2384,7 +2360,7 @@
         <v>137</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>99</v>
@@ -2398,7 +2374,7 @@
         <v>139</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>99</v>
@@ -2412,7 +2388,7 @@
         <v>141</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>99</v>
@@ -2426,7 +2402,7 @@
         <v>143</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>99</v>
@@ -2440,7 +2416,7 @@
         <v>145</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>99</v>
@@ -2454,7 +2430,7 @@
         <v>147</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>99</v>
@@ -2468,7 +2444,7 @@
         <v>149</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>99</v>
@@ -2482,7 +2458,7 @@
         <v>151</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>99</v>
@@ -2496,7 +2472,7 @@
         <v>153</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>99</v>
@@ -2510,7 +2486,7 @@
         <v>155</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>99</v>
@@ -2524,7 +2500,7 @@
         <v>157</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>99</v>
@@ -2538,7 +2514,7 @@
         <v>159</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>99</v>
@@ -2553,8 +2529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D3B5F6E-7E24-4998-96F9-B8289667BDCE}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2566,105 +2542,105 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="13" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="88.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="10" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="11" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="E4" s="14" t="s">
+    <row r="5" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>162</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made below changes 1. Added Customer related calculated fields 2. Updated Data Dictionary with the updated changes in the code and added Rules explanation 3. Added a EDA Folder and uploaded all the data summary files.
</commit_message>
<xml_diff>
--- a/Data Dictionary.xlsx
+++ b/Data Dictionary.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fc4bd521ffc22738/Desktop/Freelancing/AIGEN/smartsentry_aml_model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{4E8E6087-2FD7-42AA-9DC6-118DBB4092B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{055F9C7F-6D0C-48D7-AD23-F4A5C58C2F29}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="8_{4E8E6087-2FD7-42AA-9DC6-118DBB4092B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9719AAD8-571C-4106-9807-6FB73E7C7251}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer &amp; Account" sheetId="1" r:id="rId1"/>
     <sheet name="Transaction Data" sheetId="6" r:id="rId2"/>
     <sheet name="Typology Flags Explained" sheetId="3" r:id="rId3"/>
-    <sheet name="ER Diagram" sheetId="5" r:id="rId4"/>
+    <sheet name="AML Rule based columns Explaine" sheetId="7" r:id="rId4"/>
+    <sheet name="ER Diagram" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="445">
   <si>
     <t>column_name</t>
   </si>
@@ -715,9 +716,6 @@
     <t>System Generated</t>
   </si>
   <si>
-    <t>Not useful if it is just debit and wrt to sender side</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -743,12 +741,780 @@
 • Transfers occur within minutes.</t>
     </r>
   </si>
+  <si>
+    <t>txn_count_last_7d</t>
+  </si>
+  <si>
+    <t>ACCOUNT: Transaction count in the last 7 days.</t>
+  </si>
+  <si>
+    <t>txn_count_last_30d</t>
+  </si>
+  <si>
+    <t>ACCOUNT: Transaction count in the last 30 days.</t>
+  </si>
+  <si>
+    <t>amount_zscore_30d</t>
+  </si>
+  <si>
+    <t>ACCOUNT: Z-score of this amount vs 30-day rolling mean. &gt;3 = anomalous spike.</t>
+  </si>
+  <si>
+    <t>cust_txn_count_last_1hr</t>
+  </si>
+  <si>
+    <t>CUSTOMER: Transactions across all accounts in last 1 hour.</t>
+  </si>
+  <si>
+    <t>cust_txn_count_last_24hr</t>
+  </si>
+  <si>
+    <t>CUSTOMER: Transactions across all accounts in last 24 hours.</t>
+  </si>
+  <si>
+    <t>cust_total_amount_last_24hr</t>
+  </si>
+  <si>
+    <t>CUSTOMER: Total INR across all accounts in last 24 hours.</t>
+  </si>
+  <si>
+    <t>cust_txn_count_last_7d</t>
+  </si>
+  <si>
+    <t>CUSTOMER: Transaction count across all accounts in last 7 days.</t>
+  </si>
+  <si>
+    <t>cust_total_amount_last_7d</t>
+  </si>
+  <si>
+    <t>CUSTOMER: Total INR across all accounts in last 7 days.</t>
+  </si>
+  <si>
+    <t>cust_txn_count_last_30d</t>
+  </si>
+  <si>
+    <t>CUSTOMER: Transaction count across all accounts in last 30 days.</t>
+  </si>
+  <si>
+    <t>cust_total_amount_last_30d</t>
+  </si>
+  <si>
+    <t>CUSTOMER: Total INR across all accounts in last 30 days.</t>
+  </si>
+  <si>
+    <t>cust_unique_accounts_30d</t>
+  </si>
+  <si>
+    <t>CUSTOMER: Number of unique accounts used (cumulative proxy).</t>
+  </si>
+  <si>
+    <t>50 Rules across 10 Groups  |  Severity: 🟢 1=Low   🟡 2=Medium   🔴 3=High</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Rule Column Name</t>
+  </si>
+  <si>
+    <t>Rule (Readable)</t>
+  </si>
+  <si>
+    <t>Severity</t>
+  </si>
+  <si>
+    <t>Threshold / Condition</t>
+  </si>
+  <si>
+    <t>What It Detects</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>rule_large_cash_deposit</t>
+  </si>
+  <si>
+    <t>Large Cash Deposit</t>
+  </si>
+  <si>
+    <t>🔴 3 — High</t>
+  </si>
+  <si>
+    <t>cash_flag = 1  AND  amount &gt; ₹50,000</t>
+  </si>
+  <si>
+    <t>High-value cash deposits — placement stage of laundering</t>
+  </si>
+  <si>
+    <t>rule_cash_just_below_threshold</t>
+  </si>
+  <si>
+    <t>Cash Just Below Threshold</t>
+  </si>
+  <si>
+    <t>cash_flag = 1  AND  ₹8,000 ≤ amount ≤ ₹9,999</t>
+  </si>
+  <si>
+    <t>Cash deposits just under reporting threshold — structuring signal</t>
+  </si>
+  <si>
+    <t>rule_high_value_transfer</t>
+  </si>
+  <si>
+    <t>High Value Transfer</t>
+  </si>
+  <si>
+    <t>🟡 2 — Medium</t>
+  </si>
+  <si>
+    <t>amount &gt; ₹1,00,000</t>
+  </si>
+  <si>
+    <t>Large fund transfers regardless of type</t>
+  </si>
+  <si>
+    <t>rule_micro_transaction</t>
+  </si>
+  <si>
+    <t>Micro Transaction</t>
+  </si>
+  <si>
+    <t>🟢 1 — Low</t>
+  </si>
+  <si>
+    <t>amount &lt; ₹10</t>
+  </si>
+  <si>
+    <t>Tiny amounts — account probing or testing</t>
+  </si>
+  <si>
+    <t>rule_round_amount_large</t>
+  </si>
+  <si>
+    <t>Round Amount Large</t>
+  </si>
+  <si>
+    <t>is_round_amount = 1  AND  amount ≥ ₹10,000</t>
+  </si>
+  <si>
+    <t>Suspiciously round large amounts — common in fraud</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>rule_night_transaction</t>
+  </si>
+  <si>
+    <t>Night Transaction</t>
+  </si>
+  <si>
+    <t>is_night = 1  (10 PM – 6 AM)</t>
+  </si>
+  <si>
+    <t>Transactions outside normal hours</t>
+  </si>
+  <si>
+    <t>rule_weekend_high_value</t>
+  </si>
+  <si>
+    <t>Weekend High Value</t>
+  </si>
+  <si>
+    <t>is_weekend = 1  AND  amount &gt; ₹20,000</t>
+  </si>
+  <si>
+    <t>Large weekend transactions — lower oversight</t>
+  </si>
+  <si>
+    <t>rule_dormant_account_activation</t>
+  </si>
+  <si>
+    <t>Dormant Account Activation</t>
+  </si>
+  <si>
+    <t>dormancy_flag = 1  AND  amount &gt; ₹5,000  (gap &gt; 30 days)</t>
+  </si>
+  <si>
+    <t>Sudden activity after long inactivity</t>
+  </si>
+  <si>
+    <t>Account Velocity</t>
+  </si>
+  <si>
+    <t>rule_high_acct_velocity_1hr</t>
+  </si>
+  <si>
+    <t>High Acct Velocity 1hr</t>
+  </si>
+  <si>
+    <t>txn_count_last_1hr &gt; 5</t>
+  </si>
+  <si>
+    <t>Too many transactions in 1 hour from same account</t>
+  </si>
+  <si>
+    <t>rule_rapid_burst</t>
+  </si>
+  <si>
+    <t>Rapid Burst</t>
+  </si>
+  <si>
+    <t>txn_count_last_1hr &gt; 3</t>
+  </si>
+  <si>
+    <t>Quick burst of transactions — lower threshold early warning</t>
+  </si>
+  <si>
+    <t>rule_high_acct_velocity_24hr</t>
+  </si>
+  <si>
+    <t>High Acct Velocity 24hr</t>
+  </si>
+  <si>
+    <t>txn_count_last_24hr &gt; 20</t>
+  </si>
+  <si>
+    <t>High daily transaction count from one account</t>
+  </si>
+  <si>
+    <t>rule_high_acct_velocity_7d</t>
+  </si>
+  <si>
+    <t>High Acct Velocity 7d</t>
+  </si>
+  <si>
+    <t>txn_count_last_7d &gt; 60</t>
+  </si>
+  <si>
+    <t>High weekly transaction frequency</t>
+  </si>
+  <si>
+    <t>rule_high_acct_volume_24hr</t>
+  </si>
+  <si>
+    <t>High Acct Volume 24hr</t>
+  </si>
+  <si>
+    <t>total_amount_last_24hr &gt; ₹5,00,000</t>
+  </si>
+  <si>
+    <t>Large total amount sent in a day from one account</t>
+  </si>
+  <si>
+    <t>rule_high_acct_volume_7d</t>
+  </si>
+  <si>
+    <t>High Acct Volume 7d</t>
+  </si>
+  <si>
+    <t>total_amount_last_7d &gt; ₹20,00,000</t>
+  </si>
+  <si>
+    <t>Large total amount sent in 7 days from one account</t>
+  </si>
+  <si>
+    <t>rule_amount_spike_30d</t>
+  </si>
+  <si>
+    <t>Amount Spike 30d</t>
+  </si>
+  <si>
+    <t>amount_zscore_30d &gt; 4  (4 std deviations above mean)</t>
+  </si>
+  <si>
+    <t>This transaction is anomalously large vs account's 30-day history</t>
+  </si>
+  <si>
+    <t>Customer Velocity</t>
+  </si>
+  <si>
+    <t>rule_high_cust_velocity_1hr</t>
+  </si>
+  <si>
+    <t>High Cust Velocity 1hr</t>
+  </si>
+  <si>
+    <t>cust_txn_count_last_1hr &gt; 8</t>
+  </si>
+  <si>
+    <t>Customer transacting too fast across all accounts in 1hr</t>
+  </si>
+  <si>
+    <t>rule_high_cust_velocity_24hr</t>
+  </si>
+  <si>
+    <t>High Cust Velocity 24hr</t>
+  </si>
+  <si>
+    <t>cust_txn_count_last_24hr &gt; 30</t>
+  </si>
+  <si>
+    <t>Customer's total daily transaction count is very high</t>
+  </si>
+  <si>
+    <t>rule_high_cust_volume_24hr</t>
+  </si>
+  <si>
+    <t>High Cust Volume 24hr</t>
+  </si>
+  <si>
+    <t>cust_total_amount_last_24hr &gt; ₹10,00,000</t>
+  </si>
+  <si>
+    <t>Customer sent over ₹10L in a single day across all accounts</t>
+  </si>
+  <si>
+    <t>rule_high_cust_volume_7d</t>
+  </si>
+  <si>
+    <t>High Cust Volume 7d</t>
+  </si>
+  <si>
+    <t>cust_total_amount_last_7d &gt; ₹30,00,000</t>
+  </si>
+  <si>
+    <t>Customer sent over ₹30L in 7 days across all accounts</t>
+  </si>
+  <si>
+    <t>KYC / Account</t>
+  </si>
+  <si>
+    <t>rule_low_kyc_high_amount</t>
+  </si>
+  <si>
+    <t>Low KYC High Amount</t>
+  </si>
+  <si>
+    <t>kyc_level = 'low'  AND  amount &gt; ₹30,000</t>
+  </si>
+  <si>
+    <t>Unverified customer sending large amounts</t>
+  </si>
+  <si>
+    <t>rule_new_account_large_txn</t>
+  </si>
+  <si>
+    <t>New Account Large Txn</t>
+  </si>
+  <si>
+    <t>account_open_days &lt; 60  AND  amount &gt; ₹10,000</t>
+  </si>
+  <si>
+    <t>Brand new account (&lt;2 months) with large transactions</t>
+  </si>
+  <si>
+    <t>rule_high_amount_to_balance</t>
+  </si>
+  <si>
+    <t>High Amount to Balance</t>
+  </si>
+  <si>
+    <t>amount_to_balance_ratio &gt; 3</t>
+  </si>
+  <si>
+    <t>Transaction amount is 3× the account's average balance</t>
+  </si>
+  <si>
+    <t>rule_very_high_risk_customer</t>
+  </si>
+  <si>
+    <t>Very High Risk Customer</t>
+  </si>
+  <si>
+    <t>customer_risk_rating = 'very_high'</t>
+  </si>
+  <si>
+    <t>Customer already rated very high risk in CRM</t>
+  </si>
+  <si>
+    <t>rule_pep_high_value</t>
+  </si>
+  <si>
+    <t>PEP High Value</t>
+  </si>
+  <si>
+    <t>pep_flag = 1  AND  amount &gt; ₹10,000</t>
+  </si>
+  <si>
+    <t>Politically Exposed Person making large transaction</t>
+  </si>
+  <si>
+    <t>rule_high_risk_country_sender</t>
+  </si>
+  <si>
+    <t>High Risk Country Sender</t>
+  </si>
+  <si>
+    <t>country_risk = 'high'  (FATF grey/blacklist)</t>
+  </si>
+  <si>
+    <t>Transaction from a high-risk jurisdiction</t>
+  </si>
+  <si>
+    <t>rule_corporate_large_cash</t>
+  </si>
+  <si>
+    <t>Corporate Large Cash</t>
+  </si>
+  <si>
+    <t>account_type in (corporate, business)  AND  cash_flag=1  AND  amount &gt; ₹20,000</t>
+  </si>
+  <si>
+    <t>Corporate account using large cash — unusual</t>
+  </si>
+  <si>
+    <t>Beneficiary</t>
+  </si>
+  <si>
+    <t>rule_high_risk_beneficiary</t>
+  </si>
+  <si>
+    <t>High Risk Beneficiary</t>
+  </si>
+  <si>
+    <t>high_risk_beneficiary = 1</t>
+  </si>
+  <si>
+    <t>Beneficiary is pre-flagged as high risk</t>
+  </si>
+  <si>
+    <t>rule_crypto_transfer</t>
+  </si>
+  <si>
+    <t>Crypto Transfer</t>
+  </si>
+  <si>
+    <t>beneficiary_type = 'crypto'</t>
+  </si>
+  <si>
+    <t>Money going to a crypto wallet — high anonymity</t>
+  </si>
+  <si>
+    <t>rule_offshore_transfer</t>
+  </si>
+  <si>
+    <t>Offshore Transfer</t>
+  </si>
+  <si>
+    <t>beneficiary_type = 'offshore'</t>
+  </si>
+  <si>
+    <t>Money going offshore — cross-border laundering risk</t>
+  </si>
+  <si>
+    <t>rule_high_risk_bene_country</t>
+  </si>
+  <si>
+    <t>High Risk Bene Country</t>
+  </si>
+  <si>
+    <t>beneficiary_country_risk = 'high'</t>
+  </si>
+  <si>
+    <t>Destination country is FATF high-risk</t>
+  </si>
+  <si>
+    <t>Device / Channel</t>
+  </si>
+  <si>
+    <t>rule_rooted_device</t>
+  </si>
+  <si>
+    <t>Rooted Device</t>
+  </si>
+  <si>
+    <t>rooted_flag = 1</t>
+  </si>
+  <si>
+    <t>Device is rooted — security controls bypassed</t>
+  </si>
+  <si>
+    <t>rule_vpn_proxy_detected</t>
+  </si>
+  <si>
+    <t>VPN / Proxy Detected</t>
+  </si>
+  <si>
+    <t>vpn_flag = 1</t>
+  </si>
+  <si>
+    <t>VPN active — true location hidden</t>
+  </si>
+  <si>
+    <t>rule_emulator_detected</t>
+  </si>
+  <si>
+    <t>Emulator Detected</t>
+  </si>
+  <si>
+    <t>emulator_flag = 1</t>
+  </si>
+  <si>
+    <t>Transaction from emulator — automated fraud tool</t>
+  </si>
+  <si>
+    <t>rule_new_device_large_txn</t>
+  </si>
+  <si>
+    <t>New Device Large Txn</t>
+  </si>
+  <si>
+    <t>device_age_days &lt; 90  AND  amount &gt; ₹10,000</t>
+  </si>
+  <si>
+    <t>New device making large transaction — account takeover risk</t>
+  </si>
+  <si>
+    <t>rule_atm_high_withdrawal</t>
+  </si>
+  <si>
+    <t>ATM High Withdrawal</t>
+  </si>
+  <si>
+    <t>channel = 'atm'  AND  amount &gt; ₹20,000</t>
+  </si>
+  <si>
+    <t>Large ATM cash withdrawal</t>
+  </si>
+  <si>
+    <t>rule_branch_night_txn</t>
+  </si>
+  <si>
+    <t>Branch Night Txn</t>
+  </si>
+  <si>
+    <t>channel = 'branch'  AND  is_night = 1</t>
+  </si>
+  <si>
+    <t>In-branch transaction during night hours</t>
+  </si>
+  <si>
+    <t>Structuring</t>
+  </si>
+  <si>
+    <t>rule_structuring_pattern</t>
+  </si>
+  <si>
+    <t>Structuring Pattern</t>
+  </si>
+  <si>
+    <t>cash_flag=1  AND  ₹8,500 ≤ amount ≤ ₹9,999</t>
+  </si>
+  <si>
+    <t>Classic structuring — splitting cash just below ₹10K limit</t>
+  </si>
+  <si>
+    <t>rule_multiple_small_cash</t>
+  </si>
+  <si>
+    <t>Multiple Small Cash</t>
+  </si>
+  <si>
+    <t>cash_flag=1  AND  txn_count_last_7d &gt; 5  AND  amount &lt; ₹10,000</t>
+  </si>
+  <si>
+    <t>Repeated small cash transactions — smurfing pattern</t>
+  </si>
+  <si>
+    <t>Occupation / Industry</t>
+  </si>
+  <si>
+    <t>rule_high_risk_industry</t>
+  </si>
+  <si>
+    <t>High Risk Industry</t>
+  </si>
+  <si>
+    <t>industry in (real_estate, construction, unknown)</t>
+  </si>
+  <si>
+    <t>Industries commonly used for money laundering</t>
+  </si>
+  <si>
+    <t>rule_student_high_value</t>
+  </si>
+  <si>
+    <t>Student High Value</t>
+  </si>
+  <si>
+    <t>occupation = 'student'  AND  amount &gt; ₹50,000</t>
+  </si>
+  <si>
+    <t>Student with income-inconsistent large transaction</t>
+  </si>
+  <si>
+    <t>rule_unemployed_large_transfer</t>
+  </si>
+  <si>
+    <t>Unemployed Large Transfer</t>
+  </si>
+  <si>
+    <t>occupation = 'unemployed'  AND  amount &gt; ₹20,000</t>
+  </si>
+  <si>
+    <t>Unemployed person sending large amount — income mismatch</t>
+  </si>
+  <si>
+    <t>rule_freelancer_offshore</t>
+  </si>
+  <si>
+    <t>Freelancer Offshore</t>
+  </si>
+  <si>
+    <t>occupation = 'freelancer'  AND  beneficiary_type = 'offshore'</t>
+  </si>
+  <si>
+    <t>Freelancer routing money offshore</t>
+  </si>
+  <si>
+    <t>Combined Risk Combos</t>
+  </si>
+  <si>
+    <t>rule_pep_crypto_transfer</t>
+  </si>
+  <si>
+    <t>PEP + Crypto Transfer</t>
+  </si>
+  <si>
+    <t>pep_flag = 1  AND  beneficiary_type = 'crypto'</t>
+  </si>
+  <si>
+    <t>PEP sending to crypto — very high risk combo</t>
+  </si>
+  <si>
+    <t>rule_very_high_risk_offshore</t>
+  </si>
+  <si>
+    <t>Very High Risk + Offshore</t>
+  </si>
+  <si>
+    <t>customer_risk_rating = 'very_high'  AND  beneficiary_type = 'offshore'</t>
+  </si>
+  <si>
+    <t>Highest risk customer sending offshore</t>
+  </si>
+  <si>
+    <t>rule_low_kyc_offshore</t>
+  </si>
+  <si>
+    <t>Low KYC + Offshore</t>
+  </si>
+  <si>
+    <t>kyc_level = 'low'  AND  beneficiary_type = 'offshore'</t>
+  </si>
+  <si>
+    <t>Unverified customer sending money offshore</t>
+  </si>
+  <si>
+    <t>rule_low_income_large_txn</t>
+  </si>
+  <si>
+    <t>Low Income Large Txn</t>
+  </si>
+  <si>
+    <t>income_bracket = 'low'  AND  amount &gt; ₹50,000</t>
+  </si>
+  <si>
+    <t>Low income customer with large transaction</t>
+  </si>
+  <si>
+    <t>rule_vpn_offshore</t>
+  </si>
+  <si>
+    <t>VPN + Offshore</t>
+  </si>
+  <si>
+    <t>vpn_flag = 1  AND  beneficiary_type = 'offshore'</t>
+  </si>
+  <si>
+    <t>VPN active while sending offshore — layering signal</t>
+  </si>
+  <si>
+    <t>rule_emulator_crypto</t>
+  </si>
+  <si>
+    <t>Emulator + Crypto</t>
+  </si>
+  <si>
+    <t>emulator_flag = 1  AND  beneficiary_type = 'crypto'</t>
+  </si>
+  <si>
+    <t>Automated tool sending to crypto — bot fraud</t>
+  </si>
+  <si>
+    <t>rule_new_account_offshore</t>
+  </si>
+  <si>
+    <t>New Account + Offshore</t>
+  </si>
+  <si>
+    <t>account_open_days &lt; 90  AND  beneficiary_type = 'offshore'</t>
+  </si>
+  <si>
+    <t>Brand new account sending offshore immediately</t>
+  </si>
+  <si>
+    <t>rule_new_acct_high_cust_velocity</t>
+  </si>
+  <si>
+    <t>New Account + High Velocity</t>
+  </si>
+  <si>
+    <t>account_open_days &lt; 90  AND  cust_txn_count_last_24hr &gt; 10</t>
+  </si>
+  <si>
+    <t>New account with customer showing burst activity</t>
+  </si>
+  <si>
+    <t>📊  Aggregate Score Columns — How the 3 summary columns are computed per transaction</t>
+  </si>
+  <si>
+    <t>Column</t>
+  </si>
+  <si>
+    <t>Operation</t>
+  </si>
+  <si>
+    <t>Formula Logic</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Sum of all rule columns (0/1) for a transaction</t>
+  </si>
+  <si>
+    <t>If 4 rules fire → rule_trigger_count = 4</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Highest severity among all rules that fired</t>
+  </si>
+  <si>
+    <t>If rules of severity 2, 3, 1 fire → max_rule_severity = 3</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Sum of severities of all fired rules</t>
+  </si>
+  <si>
+    <t>If rules 3+2+1 fire → weighted_rule_score = 6</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -787,15 +1553,124 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF1A3A5C"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF1F2D3D"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF555555"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF1F2D3D"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF2C3E50"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF4A4A4A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF1A3A5C"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF1F2D3D"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF1A3A5C"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF922B21"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF9A7D0A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF1E8449"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -832,8 +1707,39 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2E75B6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFADBD8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFEF9E7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD5F5E3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF1B2631"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -878,11 +1784,71 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB8CCE4"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB8CCE4"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB8CCE4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB8CCE4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB8CCE4"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB8CCE4"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB8CCE4"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB8CCE4"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFB8CCE4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB8CCE4"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFB8CCE4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFB8CCE4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -935,15 +1901,79 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1295,8 +2325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:E35"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1309,12 +2339,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
@@ -1485,12 +2515,12 @@
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="18" t="s">
@@ -1549,12 +2579,12 @@
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="18" t="s">
@@ -1655,12 +2685,12 @@
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B31" s="21" t="s">
+      <c r="B31" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B32" s="18" t="s">
@@ -1732,22 +2762,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D359FD-D224-4E20-8A0E-46CD436ABBB7}">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31" style="4" customWidth="1"/>
     <col min="2" max="2" width="118.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.44140625" style="4" customWidth="1"/>
     <col min="4" max="4" width="12.77734375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1761,7 +2791,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>87</v>
       </c>
@@ -1775,7 +2805,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>4</v>
       </c>
@@ -1789,7 +2819,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>91</v>
       </c>
@@ -1803,7 +2833,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>93</v>
       </c>
@@ -1817,7 +2847,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>52</v>
       </c>
@@ -1831,7 +2861,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>39</v>
       </c>
@@ -1845,7 +2875,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>97</v>
       </c>
@@ -1859,7 +2889,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>100</v>
       </c>
@@ -1873,7 +2903,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>102</v>
       </c>
@@ -1887,7 +2917,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>104</v>
       </c>
@@ -1900,11 +2930,8 @@
       <c r="D11" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E11" s="20" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>106</v>
       </c>
@@ -1918,7 +2945,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>108</v>
       </c>
@@ -1932,8 +2959,8 @@
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="22" t="s">
         <v>110</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1946,7 +2973,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>112</v>
       </c>
@@ -1960,7 +2987,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>34</v>
       </c>
@@ -2520,7 +3547,164 @@
         <v>99</v>
       </c>
     </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A14" location="'Typology Flags Explained'!A1" display="fraud_type" xr:uid="{D85CD9F3-3974-4380-9C82-D288F4234166}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2529,8 +3713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D3B5F6E-7E24-4998-96F9-B8289667BDCE}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2589,7 +3773,7 @@
         <v>71</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -2649,6 +3833,1064 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8A5AEFB-10F4-4DE5-9F32-2D9D8885243B}">
+  <dimension ref="A1:F59"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" style="31" customWidth="1"/>
+    <col min="3" max="3" width="25.77734375" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" customWidth="1"/>
+    <col min="5" max="5" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+    </row>
+    <row r="2" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="30" t="s">
+        <v>218</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>219</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>220</v>
+      </c>
+      <c r="D3" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="E3" s="35" t="s">
+        <v>222</v>
+      </c>
+      <c r="F3" s="36" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="27"/>
+      <c r="B4" s="33" t="s">
+        <v>224</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>225</v>
+      </c>
+      <c r="D4" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="E4" s="35" t="s">
+        <v>226</v>
+      </c>
+      <c r="F4" s="36" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="27"/>
+      <c r="B5" s="33" t="s">
+        <v>228</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>229</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>230</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>231</v>
+      </c>
+      <c r="F5" s="36" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="27"/>
+      <c r="B6" s="33" t="s">
+        <v>233</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>234</v>
+      </c>
+      <c r="D6" s="39" t="s">
+        <v>235</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>236</v>
+      </c>
+      <c r="F6" s="36" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="28"/>
+      <c r="B7" s="33" t="s">
+        <v>238</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>239</v>
+      </c>
+      <c r="D7" s="39" t="s">
+        <v>235</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="F7" s="36" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="30" t="s">
+        <v>242</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>243</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>244</v>
+      </c>
+      <c r="D8" s="38" t="s">
+        <v>230</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>245</v>
+      </c>
+      <c r="F8" s="36" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="27"/>
+      <c r="B9" s="33" t="s">
+        <v>247</v>
+      </c>
+      <c r="C9" s="34" t="s">
+        <v>248</v>
+      </c>
+      <c r="D9" s="38" t="s">
+        <v>230</v>
+      </c>
+      <c r="E9" s="35" t="s">
+        <v>249</v>
+      </c>
+      <c r="F9" s="36" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="28"/>
+      <c r="B10" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>252</v>
+      </c>
+      <c r="D10" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>253</v>
+      </c>
+      <c r="F10" s="36" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="30" t="s">
+        <v>255</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>257</v>
+      </c>
+      <c r="D11" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>258</v>
+      </c>
+      <c r="F11" s="36" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="27"/>
+      <c r="B12" s="33" t="s">
+        <v>260</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>261</v>
+      </c>
+      <c r="D12" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>262</v>
+      </c>
+      <c r="F12" s="36" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="27"/>
+      <c r="B13" s="33" t="s">
+        <v>264</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>265</v>
+      </c>
+      <c r="D13" s="38" t="s">
+        <v>230</v>
+      </c>
+      <c r="E13" s="35" t="s">
+        <v>266</v>
+      </c>
+      <c r="F13" s="36" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="27"/>
+      <c r="B14" s="33" t="s">
+        <v>268</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>269</v>
+      </c>
+      <c r="D14" s="38" t="s">
+        <v>230</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>270</v>
+      </c>
+      <c r="F14" s="36" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="27"/>
+      <c r="B15" s="33" t="s">
+        <v>272</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>273</v>
+      </c>
+      <c r="D15" s="38" t="s">
+        <v>230</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>274</v>
+      </c>
+      <c r="F15" s="36" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="27"/>
+      <c r="B16" s="33" t="s">
+        <v>276</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>277</v>
+      </c>
+      <c r="D16" s="38" t="s">
+        <v>230</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>278</v>
+      </c>
+      <c r="F16" s="36" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="28"/>
+      <c r="B17" s="33" t="s">
+        <v>280</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>281</v>
+      </c>
+      <c r="D17" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="E17" s="35" t="s">
+        <v>282</v>
+      </c>
+      <c r="F17" s="36" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="30" t="s">
+        <v>284</v>
+      </c>
+      <c r="B18" s="33" t="s">
+        <v>285</v>
+      </c>
+      <c r="C18" s="34" t="s">
+        <v>286</v>
+      </c>
+      <c r="D18" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="E18" s="35" t="s">
+        <v>287</v>
+      </c>
+      <c r="F18" s="36" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="27"/>
+      <c r="B19" s="33" t="s">
+        <v>289</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>290</v>
+      </c>
+      <c r="D19" s="38" t="s">
+        <v>230</v>
+      </c>
+      <c r="E19" s="35" t="s">
+        <v>291</v>
+      </c>
+      <c r="F19" s="36" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="27"/>
+      <c r="B20" s="33" t="s">
+        <v>293</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>294</v>
+      </c>
+      <c r="D20" s="38" t="s">
+        <v>230</v>
+      </c>
+      <c r="E20" s="35" t="s">
+        <v>295</v>
+      </c>
+      <c r="F20" s="36" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="28"/>
+      <c r="B21" s="33" t="s">
+        <v>297</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>298</v>
+      </c>
+      <c r="D21" s="38" t="s">
+        <v>230</v>
+      </c>
+      <c r="E21" s="35" t="s">
+        <v>299</v>
+      </c>
+      <c r="F21" s="36" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="30" t="s">
+        <v>301</v>
+      </c>
+      <c r="B22" s="33" t="s">
+        <v>302</v>
+      </c>
+      <c r="C22" s="34" t="s">
+        <v>303</v>
+      </c>
+      <c r="D22" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="E22" s="35" t="s">
+        <v>304</v>
+      </c>
+      <c r="F22" s="36" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="27"/>
+      <c r="B23" s="33" t="s">
+        <v>306</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>307</v>
+      </c>
+      <c r="D23" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="E23" s="35" t="s">
+        <v>308</v>
+      </c>
+      <c r="F23" s="36" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="27"/>
+      <c r="B24" s="33" t="s">
+        <v>310</v>
+      </c>
+      <c r="C24" s="34" t="s">
+        <v>311</v>
+      </c>
+      <c r="D24" s="38" t="s">
+        <v>230</v>
+      </c>
+      <c r="E24" s="35" t="s">
+        <v>312</v>
+      </c>
+      <c r="F24" s="36" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="27"/>
+      <c r="B25" s="33" t="s">
+        <v>314</v>
+      </c>
+      <c r="C25" s="34" t="s">
+        <v>315</v>
+      </c>
+      <c r="D25" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="E25" s="35" t="s">
+        <v>316</v>
+      </c>
+      <c r="F25" s="36" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="27"/>
+      <c r="B26" s="33" t="s">
+        <v>318</v>
+      </c>
+      <c r="C26" s="34" t="s">
+        <v>319</v>
+      </c>
+      <c r="D26" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="E26" s="35" t="s">
+        <v>320</v>
+      </c>
+      <c r="F26" s="36" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="27"/>
+      <c r="B27" s="33" t="s">
+        <v>322</v>
+      </c>
+      <c r="C27" s="34" t="s">
+        <v>323</v>
+      </c>
+      <c r="D27" s="38" t="s">
+        <v>230</v>
+      </c>
+      <c r="E27" s="35" t="s">
+        <v>324</v>
+      </c>
+      <c r="F27" s="36" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="28"/>
+      <c r="B28" s="33" t="s">
+        <v>326</v>
+      </c>
+      <c r="C28" s="34" t="s">
+        <v>327</v>
+      </c>
+      <c r="D28" s="38" t="s">
+        <v>230</v>
+      </c>
+      <c r="E28" s="35" t="s">
+        <v>328</v>
+      </c>
+      <c r="F28" s="36" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="30" t="s">
+        <v>330</v>
+      </c>
+      <c r="B29" s="33" t="s">
+        <v>331</v>
+      </c>
+      <c r="C29" s="34" t="s">
+        <v>332</v>
+      </c>
+      <c r="D29" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="E29" s="35" t="s">
+        <v>333</v>
+      </c>
+      <c r="F29" s="36" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="27"/>
+      <c r="B30" s="33" t="s">
+        <v>335</v>
+      </c>
+      <c r="C30" s="34" t="s">
+        <v>336</v>
+      </c>
+      <c r="D30" s="38" t="s">
+        <v>230</v>
+      </c>
+      <c r="E30" s="35" t="s">
+        <v>337</v>
+      </c>
+      <c r="F30" s="36" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="27"/>
+      <c r="B31" s="33" t="s">
+        <v>339</v>
+      </c>
+      <c r="C31" s="34" t="s">
+        <v>340</v>
+      </c>
+      <c r="D31" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="E31" s="35" t="s">
+        <v>341</v>
+      </c>
+      <c r="F31" s="36" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="28"/>
+      <c r="B32" s="33" t="s">
+        <v>343</v>
+      </c>
+      <c r="C32" s="34" t="s">
+        <v>344</v>
+      </c>
+      <c r="D32" s="38" t="s">
+        <v>230</v>
+      </c>
+      <c r="E32" s="35" t="s">
+        <v>345</v>
+      </c>
+      <c r="F32" s="36" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="30" t="s">
+        <v>347</v>
+      </c>
+      <c r="B33" s="33" t="s">
+        <v>348</v>
+      </c>
+      <c r="C33" s="34" t="s">
+        <v>349</v>
+      </c>
+      <c r="D33" s="38" t="s">
+        <v>230</v>
+      </c>
+      <c r="E33" s="35" t="s">
+        <v>350</v>
+      </c>
+      <c r="F33" s="36" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="27"/>
+      <c r="B34" s="33" t="s">
+        <v>352</v>
+      </c>
+      <c r="C34" s="34" t="s">
+        <v>353</v>
+      </c>
+      <c r="D34" s="38" t="s">
+        <v>230</v>
+      </c>
+      <c r="E34" s="35" t="s">
+        <v>354</v>
+      </c>
+      <c r="F34" s="36" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="27"/>
+      <c r="B35" s="33" t="s">
+        <v>356</v>
+      </c>
+      <c r="C35" s="34" t="s">
+        <v>357</v>
+      </c>
+      <c r="D35" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="E35" s="35" t="s">
+        <v>358</v>
+      </c>
+      <c r="F35" s="36" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="27"/>
+      <c r="B36" s="33" t="s">
+        <v>360</v>
+      </c>
+      <c r="C36" s="34" t="s">
+        <v>361</v>
+      </c>
+      <c r="D36" s="39" t="s">
+        <v>235</v>
+      </c>
+      <c r="E36" s="35" t="s">
+        <v>362</v>
+      </c>
+      <c r="F36" s="36" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="27"/>
+      <c r="B37" s="33" t="s">
+        <v>364</v>
+      </c>
+      <c r="C37" s="34" t="s">
+        <v>365</v>
+      </c>
+      <c r="D37" s="38" t="s">
+        <v>230</v>
+      </c>
+      <c r="E37" s="35" t="s">
+        <v>366</v>
+      </c>
+      <c r="F37" s="36" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="28"/>
+      <c r="B38" s="33" t="s">
+        <v>368</v>
+      </c>
+      <c r="C38" s="34" t="s">
+        <v>369</v>
+      </c>
+      <c r="D38" s="38" t="s">
+        <v>230</v>
+      </c>
+      <c r="E38" s="35" t="s">
+        <v>370</v>
+      </c>
+      <c r="F38" s="36" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="30" t="s">
+        <v>372</v>
+      </c>
+      <c r="B39" s="33" t="s">
+        <v>373</v>
+      </c>
+      <c r="C39" s="34" t="s">
+        <v>374</v>
+      </c>
+      <c r="D39" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="E39" s="35" t="s">
+        <v>375</v>
+      </c>
+      <c r="F39" s="36" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="28"/>
+      <c r="B40" s="33" t="s">
+        <v>377</v>
+      </c>
+      <c r="C40" s="34" t="s">
+        <v>378</v>
+      </c>
+      <c r="D40" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="E40" s="35" t="s">
+        <v>379</v>
+      </c>
+      <c r="F40" s="36" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="30" t="s">
+        <v>381</v>
+      </c>
+      <c r="B41" s="33" t="s">
+        <v>382</v>
+      </c>
+      <c r="C41" s="34" t="s">
+        <v>383</v>
+      </c>
+      <c r="D41" s="39" t="s">
+        <v>235</v>
+      </c>
+      <c r="E41" s="35" t="s">
+        <v>384</v>
+      </c>
+      <c r="F41" s="36" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="27"/>
+      <c r="B42" s="33" t="s">
+        <v>386</v>
+      </c>
+      <c r="C42" s="34" t="s">
+        <v>387</v>
+      </c>
+      <c r="D42" s="38" t="s">
+        <v>230</v>
+      </c>
+      <c r="E42" s="35" t="s">
+        <v>388</v>
+      </c>
+      <c r="F42" s="36" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="27"/>
+      <c r="B43" s="33" t="s">
+        <v>390</v>
+      </c>
+      <c r="C43" s="34" t="s">
+        <v>391</v>
+      </c>
+      <c r="D43" s="38" t="s">
+        <v>230</v>
+      </c>
+      <c r="E43" s="35" t="s">
+        <v>392</v>
+      </c>
+      <c r="F43" s="36" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="28"/>
+      <c r="B44" s="33" t="s">
+        <v>394</v>
+      </c>
+      <c r="C44" s="34" t="s">
+        <v>395</v>
+      </c>
+      <c r="D44" s="38" t="s">
+        <v>230</v>
+      </c>
+      <c r="E44" s="35" t="s">
+        <v>396</v>
+      </c>
+      <c r="F44" s="36" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="30" t="s">
+        <v>398</v>
+      </c>
+      <c r="B45" s="33" t="s">
+        <v>399</v>
+      </c>
+      <c r="C45" s="34" t="s">
+        <v>400</v>
+      </c>
+      <c r="D45" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="E45" s="35" t="s">
+        <v>401</v>
+      </c>
+      <c r="F45" s="36" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="27"/>
+      <c r="B46" s="33" t="s">
+        <v>403</v>
+      </c>
+      <c r="C46" s="34" t="s">
+        <v>404</v>
+      </c>
+      <c r="D46" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="E46" s="35" t="s">
+        <v>405</v>
+      </c>
+      <c r="F46" s="36" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="27"/>
+      <c r="B47" s="33" t="s">
+        <v>407</v>
+      </c>
+      <c r="C47" s="34" t="s">
+        <v>408</v>
+      </c>
+      <c r="D47" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="E47" s="35" t="s">
+        <v>409</v>
+      </c>
+      <c r="F47" s="36" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="27"/>
+      <c r="B48" s="33" t="s">
+        <v>411</v>
+      </c>
+      <c r="C48" s="34" t="s">
+        <v>412</v>
+      </c>
+      <c r="D48" s="38" t="s">
+        <v>230</v>
+      </c>
+      <c r="E48" s="35" t="s">
+        <v>413</v>
+      </c>
+      <c r="F48" s="36" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="27"/>
+      <c r="B49" s="33" t="s">
+        <v>415</v>
+      </c>
+      <c r="C49" s="34" t="s">
+        <v>416</v>
+      </c>
+      <c r="D49" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="E49" s="35" t="s">
+        <v>417</v>
+      </c>
+      <c r="F49" s="36" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="27"/>
+      <c r="B50" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="C50" s="34" t="s">
+        <v>420</v>
+      </c>
+      <c r="D50" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="E50" s="35" t="s">
+        <v>421</v>
+      </c>
+      <c r="F50" s="36" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="27"/>
+      <c r="B51" s="33" t="s">
+        <v>423</v>
+      </c>
+      <c r="C51" s="34" t="s">
+        <v>424</v>
+      </c>
+      <c r="D51" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="E51" s="35" t="s">
+        <v>425</v>
+      </c>
+      <c r="F51" s="36" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="28"/>
+      <c r="B52" s="33" t="s">
+        <v>427</v>
+      </c>
+      <c r="C52" s="34" t="s">
+        <v>428</v>
+      </c>
+      <c r="D52" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="E52" s="35" t="s">
+        <v>429</v>
+      </c>
+      <c r="F52" s="36" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D53" s="5"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D54" s="5"/>
+    </row>
+    <row r="55" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="25" t="s">
+        <v>431</v>
+      </c>
+      <c r="B55" s="26"/>
+      <c r="C55" s="26"/>
+      <c r="D55" s="26"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" s="23" t="s">
+        <v>432</v>
+      </c>
+      <c r="B56" s="32" t="s">
+        <v>433</v>
+      </c>
+      <c r="C56" s="24" t="s">
+        <v>434</v>
+      </c>
+      <c r="D56" s="23" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="41" t="s">
+        <v>154</v>
+      </c>
+      <c r="B57" s="42" t="s">
+        <v>436</v>
+      </c>
+      <c r="C57" s="43" t="s">
+        <v>437</v>
+      </c>
+      <c r="D57" s="44" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="45" t="s">
+        <v>156</v>
+      </c>
+      <c r="B58" s="42" t="s">
+        <v>439</v>
+      </c>
+      <c r="C58" s="43" t="s">
+        <v>440</v>
+      </c>
+      <c r="D58" s="44" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="45" t="s">
+        <v>158</v>
+      </c>
+      <c r="B59" s="42" t="s">
+        <v>442</v>
+      </c>
+      <c r="C59" s="43" t="s">
+        <v>443</v>
+      </c>
+      <c r="D59" s="44" t="s">
+        <v>444</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A33:A38"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A52"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A17"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A22:A28"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05793ECF-E58E-457E-A020-3AA8EA0E9356}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
1. Updated code with additional feature calculations, EDA codes for each data generation code is updated. 2. Added AML feature explanation for new features in the folder 3. Created an example for each fraud type from the transactions generated and uploaded it in EDA code 4. Pushed all the older codes in Old code folder for tracking
</commit_message>
<xml_diff>
--- a/Data Dictionary.xlsx
+++ b/Data Dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fc4bd521ffc22738/Desktop/Freelancing/AIGEN/smartsentry_aml_model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="8_{4E8E6087-2FD7-42AA-9DC6-118DBB4092B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9719AAD8-571C-4106-9807-6FB73E7C7251}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="8_{4E8E6087-2FD7-42AA-9DC6-118DBB4092B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB3DB712-DA46-4F18-BCAE-8674BB146D24}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer &amp; Account" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="455">
   <si>
     <t>column_name</t>
   </si>
@@ -1508,6 +1508,36 @@
   </si>
   <si>
     <t>If rules 3+2+1 fire → weighted_rule_score = 6</t>
+  </si>
+  <si>
+    <t>Layering (Linear + Loop)</t>
+  </si>
+  <si>
+    <t>A dormant (inactive &gt; 30 days) account is taken over by a fraudster using a new, unrecognised device. The reactivation burst — large amounts sent to high-risk beneficiaries immediately after a long silence — is a strong AML signal combining account takeover and dormancy reactivation.</t>
+  </si>
+  <si>
+    <t>Dormant Account Takeover</t>
+  </si>
+  <si>
+    <t>Dormant Account Smurfing</t>
+  </si>
+  <si>
+    <t>A reactivated dormant account is used for cash structuring: multiple cash transactions just below the ₹10,000 threshold within a few days of the reactivation event. The combination of dormancy + structuring is one of the highest-priority FATF red flags.</t>
+  </si>
+  <si>
+    <t>Dormant Account — Offshore Wire</t>
+  </si>
+  <si>
+    <t>Funds parked in a dormant account are suddenly wired offshore or to a crypto wallet immediately upon reactivation. This represents the integration step of a laundering scheme: the account was dormant during placement/layering and is now used for extraction.</t>
+  </si>
+  <si>
+    <t>New device login by an in-active user</t>
+  </si>
+  <si>
+    <t>Below-threshold cash txns (by in-active user)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wired offshore or to a crypto wallet </t>
   </si>
 </sst>
 </file>
@@ -1848,7 +1878,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1881,9 +1911,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1892,20 +1919,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1916,21 +1934,6 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1955,7 +1958,6 @@
     <xf numFmtId="0" fontId="22" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1970,6 +1972,39 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2036,6 +2071,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2325,7 +2364,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:E35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
@@ -2339,12 +2378,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
@@ -2515,24 +2554,24 @@
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="E17" s="17" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2579,24 +2618,24 @@
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D23" s="18" t="s">
+      <c r="D23" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E23" s="19" t="s">
+      <c r="E23" s="17" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2685,24 +2724,24 @@
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C32" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D32" s="18" t="s">
+      <c r="D32" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E32" s="19" t="s">
+      <c r="E32" s="17" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2795,7 +2834,7 @@
       <c r="A2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>88</v>
       </c>
       <c r="C2" s="8" t="s">
@@ -2806,72 +2845,72 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="14" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="14" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="14" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="14" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2960,7 +2999,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="18" t="s">
         <v>110</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -3711,10 +3750,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D3B5F6E-7E24-4998-96F9-B8289667BDCE}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3726,33 +3765,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="44" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="88.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="45" t="s">
         <v>70</v>
       </c>
       <c r="E2" s="10" t="s">
@@ -3760,33 +3799,33 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="D3" s="12" t="s">
-        <v>71</v>
+      <c r="D3" s="45" t="s">
+        <v>445</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="45" t="s">
         <v>77</v>
       </c>
       <c r="E4" s="11" t="s">
@@ -3794,16 +3833,16 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="45" t="s">
         <v>81</v>
       </c>
       <c r="E5" s="11" t="s">
@@ -3811,20 +3850,71 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="45" t="s">
         <v>84</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="45" t="s">
         <v>81</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>162</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="43" t="s">
+        <v>447</v>
+      </c>
+      <c r="B7" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="45" t="s">
+        <v>452</v>
+      </c>
+      <c r="D7" s="45" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" s="46" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="43" t="s">
+        <v>448</v>
+      </c>
+      <c r="B8" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="45" t="s">
+        <v>453</v>
+      </c>
+      <c r="D8" s="45" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" s="46" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="43" t="s">
+        <v>450</v>
+      </c>
+      <c r="B9" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="45" t="s">
+        <v>454</v>
+      </c>
+      <c r="D9" s="45" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="46" t="s">
+        <v>451</v>
       </c>
     </row>
   </sheetData>
@@ -3836,14 +3926,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8A5AEFB-10F4-4DE5-9F32-2D9D8885243B}">
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A46" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" style="31" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
     <col min="3" max="3" width="25.77734375" customWidth="1"/>
     <col min="4" max="4" width="29.6640625" customWidth="1"/>
     <col min="5" max="5" width="32.6640625" bestFit="1" customWidth="1"/>
@@ -3851,952 +3941,952 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="41" t="s">
         <v>211</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
     </row>
     <row r="2" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>212</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>213</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="12" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="36" t="s">
         <v>218</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="23" t="s">
         <v>220</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="24" t="s">
         <v>222</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="25" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="27"/>
-      <c r="B4" s="33" t="s">
+      <c r="A4" s="37"/>
+      <c r="B4" s="22" t="s">
         <v>224</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="23" t="s">
         <v>225</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="24" t="s">
         <v>226</v>
       </c>
-      <c r="F4" s="36" t="s">
+      <c r="F4" s="25" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="27"/>
-      <c r="B5" s="33" t="s">
+      <c r="A5" s="37"/>
+      <c r="B5" s="22" t="s">
         <v>228</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="23" t="s">
         <v>229</v>
       </c>
-      <c r="D5" s="38" t="s">
+      <c r="D5" s="27" t="s">
         <v>230</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="24" t="s">
         <v>231</v>
       </c>
-      <c r="F5" s="36" t="s">
+      <c r="F5" s="25" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="27"/>
-      <c r="B6" s="33" t="s">
+      <c r="A6" s="37"/>
+      <c r="B6" s="22" t="s">
         <v>233</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="23" t="s">
         <v>234</v>
       </c>
-      <c r="D6" s="39" t="s">
+      <c r="D6" s="28" t="s">
         <v>235</v>
       </c>
-      <c r="E6" s="35" t="s">
+      <c r="E6" s="24" t="s">
         <v>236</v>
       </c>
-      <c r="F6" s="36" t="s">
+      <c r="F6" s="25" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="28"/>
-      <c r="B7" s="33" t="s">
+      <c r="A7" s="38"/>
+      <c r="B7" s="22" t="s">
         <v>238</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="23" t="s">
         <v>239</v>
       </c>
-      <c r="D7" s="39" t="s">
+      <c r="D7" s="28" t="s">
         <v>235</v>
       </c>
-      <c r="E7" s="35" t="s">
+      <c r="E7" s="24" t="s">
         <v>240</v>
       </c>
-      <c r="F7" s="36" t="s">
+      <c r="F7" s="25" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="36" t="s">
         <v>242</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="22" t="s">
         <v>243</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="23" t="s">
         <v>244</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="D8" s="27" t="s">
         <v>230</v>
       </c>
-      <c r="E8" s="35" t="s">
+      <c r="E8" s="24" t="s">
         <v>245</v>
       </c>
-      <c r="F8" s="36" t="s">
+      <c r="F8" s="25" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="27"/>
-      <c r="B9" s="33" t="s">
+      <c r="A9" s="37"/>
+      <c r="B9" s="22" t="s">
         <v>247</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="23" t="s">
         <v>248</v>
       </c>
-      <c r="D9" s="38" t="s">
+      <c r="D9" s="27" t="s">
         <v>230</v>
       </c>
-      <c r="E9" s="35" t="s">
+      <c r="E9" s="24" t="s">
         <v>249</v>
       </c>
-      <c r="F9" s="36" t="s">
+      <c r="F9" s="25" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="28"/>
-      <c r="B10" s="33" t="s">
+      <c r="A10" s="38"/>
+      <c r="B10" s="22" t="s">
         <v>251</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="23" t="s">
         <v>252</v>
       </c>
-      <c r="D10" s="37" t="s">
+      <c r="D10" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="E10" s="35" t="s">
+      <c r="E10" s="24" t="s">
         <v>253</v>
       </c>
-      <c r="F10" s="36" t="s">
+      <c r="F10" s="25" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="36" t="s">
         <v>255</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="22" t="s">
         <v>256</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="23" t="s">
         <v>257</v>
       </c>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="E11" s="35" t="s">
+      <c r="E11" s="24" t="s">
         <v>258</v>
       </c>
-      <c r="F11" s="36" t="s">
+      <c r="F11" s="25" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="27"/>
-      <c r="B12" s="33" t="s">
+      <c r="A12" s="37"/>
+      <c r="B12" s="22" t="s">
         <v>260</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="23" t="s">
         <v>261</v>
       </c>
-      <c r="D12" s="37" t="s">
+      <c r="D12" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="E12" s="35" t="s">
+      <c r="E12" s="24" t="s">
         <v>262</v>
       </c>
-      <c r="F12" s="36" t="s">
+      <c r="F12" s="25" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="27"/>
-      <c r="B13" s="33" t="s">
+      <c r="A13" s="37"/>
+      <c r="B13" s="22" t="s">
         <v>264</v>
       </c>
-      <c r="C13" s="34" t="s">
+      <c r="C13" s="23" t="s">
         <v>265</v>
       </c>
-      <c r="D13" s="38" t="s">
+      <c r="D13" s="27" t="s">
         <v>230</v>
       </c>
-      <c r="E13" s="35" t="s">
+      <c r="E13" s="24" t="s">
         <v>266</v>
       </c>
-      <c r="F13" s="36" t="s">
+      <c r="F13" s="25" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="27"/>
-      <c r="B14" s="33" t="s">
+      <c r="A14" s="37"/>
+      <c r="B14" s="22" t="s">
         <v>268</v>
       </c>
-      <c r="C14" s="34" t="s">
+      <c r="C14" s="23" t="s">
         <v>269</v>
       </c>
-      <c r="D14" s="38" t="s">
+      <c r="D14" s="27" t="s">
         <v>230</v>
       </c>
-      <c r="E14" s="35" t="s">
+      <c r="E14" s="24" t="s">
         <v>270</v>
       </c>
-      <c r="F14" s="36" t="s">
+      <c r="F14" s="25" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="27"/>
-      <c r="B15" s="33" t="s">
+      <c r="A15" s="37"/>
+      <c r="B15" s="22" t="s">
         <v>272</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="23" t="s">
         <v>273</v>
       </c>
-      <c r="D15" s="38" t="s">
+      <c r="D15" s="27" t="s">
         <v>230</v>
       </c>
-      <c r="E15" s="35" t="s">
+      <c r="E15" s="24" t="s">
         <v>274</v>
       </c>
-      <c r="F15" s="36" t="s">
+      <c r="F15" s="25" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="27"/>
-      <c r="B16" s="33" t="s">
+      <c r="A16" s="37"/>
+      <c r="B16" s="22" t="s">
         <v>276</v>
       </c>
-      <c r="C16" s="34" t="s">
+      <c r="C16" s="23" t="s">
         <v>277</v>
       </c>
-      <c r="D16" s="38" t="s">
+      <c r="D16" s="27" t="s">
         <v>230</v>
       </c>
-      <c r="E16" s="35" t="s">
+      <c r="E16" s="24" t="s">
         <v>278</v>
       </c>
-      <c r="F16" s="36" t="s">
+      <c r="F16" s="25" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="28"/>
-      <c r="B17" s="33" t="s">
+      <c r="A17" s="38"/>
+      <c r="B17" s="22" t="s">
         <v>280</v>
       </c>
-      <c r="C17" s="34" t="s">
+      <c r="C17" s="23" t="s">
         <v>281</v>
       </c>
-      <c r="D17" s="37" t="s">
+      <c r="D17" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="E17" s="35" t="s">
+      <c r="E17" s="24" t="s">
         <v>282</v>
       </c>
-      <c r="F17" s="36" t="s">
+      <c r="F17" s="25" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="36" t="s">
         <v>284</v>
       </c>
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="22" t="s">
         <v>285</v>
       </c>
-      <c r="C18" s="34" t="s">
+      <c r="C18" s="23" t="s">
         <v>286</v>
       </c>
-      <c r="D18" s="37" t="s">
+      <c r="D18" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="E18" s="35" t="s">
+      <c r="E18" s="24" t="s">
         <v>287</v>
       </c>
-      <c r="F18" s="36" t="s">
+      <c r="F18" s="25" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="27"/>
-      <c r="B19" s="33" t="s">
+      <c r="A19" s="37"/>
+      <c r="B19" s="22" t="s">
         <v>289</v>
       </c>
-      <c r="C19" s="34" t="s">
+      <c r="C19" s="23" t="s">
         <v>290</v>
       </c>
-      <c r="D19" s="38" t="s">
+      <c r="D19" s="27" t="s">
         <v>230</v>
       </c>
-      <c r="E19" s="35" t="s">
+      <c r="E19" s="24" t="s">
         <v>291</v>
       </c>
-      <c r="F19" s="36" t="s">
+      <c r="F19" s="25" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="27"/>
-      <c r="B20" s="33" t="s">
+      <c r="A20" s="37"/>
+      <c r="B20" s="22" t="s">
         <v>293</v>
       </c>
-      <c r="C20" s="34" t="s">
+      <c r="C20" s="23" t="s">
         <v>294</v>
       </c>
-      <c r="D20" s="38" t="s">
+      <c r="D20" s="27" t="s">
         <v>230</v>
       </c>
-      <c r="E20" s="35" t="s">
+      <c r="E20" s="24" t="s">
         <v>295</v>
       </c>
-      <c r="F20" s="36" t="s">
+      <c r="F20" s="25" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="28"/>
-      <c r="B21" s="33" t="s">
+      <c r="A21" s="38"/>
+      <c r="B21" s="22" t="s">
         <v>297</v>
       </c>
-      <c r="C21" s="34" t="s">
+      <c r="C21" s="23" t="s">
         <v>298</v>
       </c>
-      <c r="D21" s="38" t="s">
+      <c r="D21" s="27" t="s">
         <v>230</v>
       </c>
-      <c r="E21" s="35" t="s">
+      <c r="E21" s="24" t="s">
         <v>299</v>
       </c>
-      <c r="F21" s="36" t="s">
+      <c r="F21" s="25" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="30" t="s">
+      <c r="A22" s="36" t="s">
         <v>301</v>
       </c>
-      <c r="B22" s="33" t="s">
+      <c r="B22" s="22" t="s">
         <v>302</v>
       </c>
-      <c r="C22" s="34" t="s">
+      <c r="C22" s="23" t="s">
         <v>303</v>
       </c>
-      <c r="D22" s="37" t="s">
+      <c r="D22" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="E22" s="35" t="s">
+      <c r="E22" s="24" t="s">
         <v>304</v>
       </c>
-      <c r="F22" s="36" t="s">
+      <c r="F22" s="25" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="27"/>
-      <c r="B23" s="33" t="s">
+      <c r="A23" s="37"/>
+      <c r="B23" s="22" t="s">
         <v>306</v>
       </c>
-      <c r="C23" s="34" t="s">
+      <c r="C23" s="23" t="s">
         <v>307</v>
       </c>
-      <c r="D23" s="37" t="s">
+      <c r="D23" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="E23" s="35" t="s">
+      <c r="E23" s="24" t="s">
         <v>308</v>
       </c>
-      <c r="F23" s="36" t="s">
+      <c r="F23" s="25" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="27"/>
-      <c r="B24" s="33" t="s">
+      <c r="A24" s="37"/>
+      <c r="B24" s="22" t="s">
         <v>310</v>
       </c>
-      <c r="C24" s="34" t="s">
+      <c r="C24" s="23" t="s">
         <v>311</v>
       </c>
-      <c r="D24" s="38" t="s">
+      <c r="D24" s="27" t="s">
         <v>230</v>
       </c>
-      <c r="E24" s="35" t="s">
+      <c r="E24" s="24" t="s">
         <v>312</v>
       </c>
-      <c r="F24" s="36" t="s">
+      <c r="F24" s="25" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="27"/>
-      <c r="B25" s="33" t="s">
+      <c r="A25" s="37"/>
+      <c r="B25" s="22" t="s">
         <v>314</v>
       </c>
-      <c r="C25" s="34" t="s">
+      <c r="C25" s="23" t="s">
         <v>315</v>
       </c>
-      <c r="D25" s="37" t="s">
+      <c r="D25" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="E25" s="35" t="s">
+      <c r="E25" s="24" t="s">
         <v>316</v>
       </c>
-      <c r="F25" s="36" t="s">
+      <c r="F25" s="25" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="27"/>
-      <c r="B26" s="33" t="s">
+      <c r="A26" s="37"/>
+      <c r="B26" s="22" t="s">
         <v>318</v>
       </c>
-      <c r="C26" s="34" t="s">
+      <c r="C26" s="23" t="s">
         <v>319</v>
       </c>
-      <c r="D26" s="37" t="s">
+      <c r="D26" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="E26" s="35" t="s">
+      <c r="E26" s="24" t="s">
         <v>320</v>
       </c>
-      <c r="F26" s="36" t="s">
+      <c r="F26" s="25" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="27"/>
-      <c r="B27" s="33" t="s">
+      <c r="A27" s="37"/>
+      <c r="B27" s="22" t="s">
         <v>322</v>
       </c>
-      <c r="C27" s="34" t="s">
+      <c r="C27" s="23" t="s">
         <v>323</v>
       </c>
-      <c r="D27" s="38" t="s">
+      <c r="D27" s="27" t="s">
         <v>230</v>
       </c>
-      <c r="E27" s="35" t="s">
+      <c r="E27" s="24" t="s">
         <v>324</v>
       </c>
-      <c r="F27" s="36" t="s">
+      <c r="F27" s="25" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="28"/>
-      <c r="B28" s="33" t="s">
+      <c r="A28" s="38"/>
+      <c r="B28" s="22" t="s">
         <v>326</v>
       </c>
-      <c r="C28" s="34" t="s">
+      <c r="C28" s="23" t="s">
         <v>327</v>
       </c>
-      <c r="D28" s="38" t="s">
+      <c r="D28" s="27" t="s">
         <v>230</v>
       </c>
-      <c r="E28" s="35" t="s">
+      <c r="E28" s="24" t="s">
         <v>328</v>
       </c>
-      <c r="F28" s="36" t="s">
+      <c r="F28" s="25" t="s">
         <v>329</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="30" t="s">
+      <c r="A29" s="36" t="s">
         <v>330</v>
       </c>
-      <c r="B29" s="33" t="s">
+      <c r="B29" s="22" t="s">
         <v>331</v>
       </c>
-      <c r="C29" s="34" t="s">
+      <c r="C29" s="23" t="s">
         <v>332</v>
       </c>
-      <c r="D29" s="37" t="s">
+      <c r="D29" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="E29" s="35" t="s">
+      <c r="E29" s="24" t="s">
         <v>333</v>
       </c>
-      <c r="F29" s="36" t="s">
+      <c r="F29" s="25" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="27"/>
-      <c r="B30" s="33" t="s">
+      <c r="A30" s="37"/>
+      <c r="B30" s="22" t="s">
         <v>335</v>
       </c>
-      <c r="C30" s="34" t="s">
+      <c r="C30" s="23" t="s">
         <v>336</v>
       </c>
-      <c r="D30" s="38" t="s">
+      <c r="D30" s="27" t="s">
         <v>230</v>
       </c>
-      <c r="E30" s="35" t="s">
+      <c r="E30" s="24" t="s">
         <v>337</v>
       </c>
-      <c r="F30" s="36" t="s">
+      <c r="F30" s="25" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="27"/>
-      <c r="B31" s="33" t="s">
+      <c r="A31" s="37"/>
+      <c r="B31" s="22" t="s">
         <v>339</v>
       </c>
-      <c r="C31" s="34" t="s">
+      <c r="C31" s="23" t="s">
         <v>340</v>
       </c>
-      <c r="D31" s="37" t="s">
+      <c r="D31" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="E31" s="35" t="s">
+      <c r="E31" s="24" t="s">
         <v>341</v>
       </c>
-      <c r="F31" s="36" t="s">
+      <c r="F31" s="25" t="s">
         <v>342</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="28"/>
-      <c r="B32" s="33" t="s">
+      <c r="A32" s="38"/>
+      <c r="B32" s="22" t="s">
         <v>343</v>
       </c>
-      <c r="C32" s="34" t="s">
+      <c r="C32" s="23" t="s">
         <v>344</v>
       </c>
-      <c r="D32" s="38" t="s">
+      <c r="D32" s="27" t="s">
         <v>230</v>
       </c>
-      <c r="E32" s="35" t="s">
+      <c r="E32" s="24" t="s">
         <v>345</v>
       </c>
-      <c r="F32" s="36" t="s">
+      <c r="F32" s="25" t="s">
         <v>346</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="30" t="s">
+      <c r="A33" s="36" t="s">
         <v>347</v>
       </c>
-      <c r="B33" s="33" t="s">
+      <c r="B33" s="22" t="s">
         <v>348</v>
       </c>
-      <c r="C33" s="34" t="s">
+      <c r="C33" s="23" t="s">
         <v>349</v>
       </c>
-      <c r="D33" s="38" t="s">
+      <c r="D33" s="27" t="s">
         <v>230</v>
       </c>
-      <c r="E33" s="35" t="s">
+      <c r="E33" s="24" t="s">
         <v>350</v>
       </c>
-      <c r="F33" s="36" t="s">
+      <c r="F33" s="25" t="s">
         <v>351</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="27"/>
-      <c r="B34" s="33" t="s">
+      <c r="A34" s="37"/>
+      <c r="B34" s="22" t="s">
         <v>352</v>
       </c>
-      <c r="C34" s="34" t="s">
+      <c r="C34" s="23" t="s">
         <v>353</v>
       </c>
-      <c r="D34" s="38" t="s">
+      <c r="D34" s="27" t="s">
         <v>230</v>
       </c>
-      <c r="E34" s="35" t="s">
+      <c r="E34" s="24" t="s">
         <v>354</v>
       </c>
-      <c r="F34" s="36" t="s">
+      <c r="F34" s="25" t="s">
         <v>355</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="27"/>
-      <c r="B35" s="33" t="s">
+      <c r="A35" s="37"/>
+      <c r="B35" s="22" t="s">
         <v>356</v>
       </c>
-      <c r="C35" s="34" t="s">
+      <c r="C35" s="23" t="s">
         <v>357</v>
       </c>
-      <c r="D35" s="37" t="s">
+      <c r="D35" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="E35" s="35" t="s">
+      <c r="E35" s="24" t="s">
         <v>358</v>
       </c>
-      <c r="F35" s="36" t="s">
+      <c r="F35" s="25" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="27"/>
-      <c r="B36" s="33" t="s">
+      <c r="A36" s="37"/>
+      <c r="B36" s="22" t="s">
         <v>360</v>
       </c>
-      <c r="C36" s="34" t="s">
+      <c r="C36" s="23" t="s">
         <v>361</v>
       </c>
-      <c r="D36" s="39" t="s">
+      <c r="D36" s="28" t="s">
         <v>235</v>
       </c>
-      <c r="E36" s="35" t="s">
+      <c r="E36" s="24" t="s">
         <v>362</v>
       </c>
-      <c r="F36" s="36" t="s">
+      <c r="F36" s="25" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="27"/>
-      <c r="B37" s="33" t="s">
+      <c r="A37" s="37"/>
+      <c r="B37" s="22" t="s">
         <v>364</v>
       </c>
-      <c r="C37" s="34" t="s">
+      <c r="C37" s="23" t="s">
         <v>365</v>
       </c>
-      <c r="D37" s="38" t="s">
+      <c r="D37" s="27" t="s">
         <v>230</v>
       </c>
-      <c r="E37" s="35" t="s">
+      <c r="E37" s="24" t="s">
         <v>366</v>
       </c>
-      <c r="F37" s="36" t="s">
+      <c r="F37" s="25" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="28"/>
-      <c r="B38" s="33" t="s">
+      <c r="A38" s="38"/>
+      <c r="B38" s="22" t="s">
         <v>368</v>
       </c>
-      <c r="C38" s="34" t="s">
+      <c r="C38" s="23" t="s">
         <v>369</v>
       </c>
-      <c r="D38" s="38" t="s">
+      <c r="D38" s="27" t="s">
         <v>230</v>
       </c>
-      <c r="E38" s="35" t="s">
+      <c r="E38" s="24" t="s">
         <v>370</v>
       </c>
-      <c r="F38" s="36" t="s">
+      <c r="F38" s="25" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="30" t="s">
+      <c r="A39" s="36" t="s">
         <v>372</v>
       </c>
-      <c r="B39" s="33" t="s">
+      <c r="B39" s="22" t="s">
         <v>373</v>
       </c>
-      <c r="C39" s="34" t="s">
+      <c r="C39" s="23" t="s">
         <v>374</v>
       </c>
-      <c r="D39" s="37" t="s">
+      <c r="D39" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="E39" s="35" t="s">
+      <c r="E39" s="24" t="s">
         <v>375</v>
       </c>
-      <c r="F39" s="36" t="s">
+      <c r="F39" s="25" t="s">
         <v>376</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="28"/>
-      <c r="B40" s="33" t="s">
+      <c r="A40" s="38"/>
+      <c r="B40" s="22" t="s">
         <v>377</v>
       </c>
-      <c r="C40" s="34" t="s">
+      <c r="C40" s="23" t="s">
         <v>378</v>
       </c>
-      <c r="D40" s="37" t="s">
+      <c r="D40" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="E40" s="35" t="s">
+      <c r="E40" s="24" t="s">
         <v>379</v>
       </c>
-      <c r="F40" s="36" t="s">
+      <c r="F40" s="25" t="s">
         <v>380</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="30" t="s">
+      <c r="A41" s="36" t="s">
         <v>381</v>
       </c>
-      <c r="B41" s="33" t="s">
+      <c r="B41" s="22" t="s">
         <v>382</v>
       </c>
-      <c r="C41" s="34" t="s">
+      <c r="C41" s="23" t="s">
         <v>383</v>
       </c>
-      <c r="D41" s="39" t="s">
+      <c r="D41" s="28" t="s">
         <v>235</v>
       </c>
-      <c r="E41" s="35" t="s">
+      <c r="E41" s="24" t="s">
         <v>384</v>
       </c>
-      <c r="F41" s="36" t="s">
+      <c r="F41" s="25" t="s">
         <v>385</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="27"/>
-      <c r="B42" s="33" t="s">
+      <c r="A42" s="37"/>
+      <c r="B42" s="22" t="s">
         <v>386</v>
       </c>
-      <c r="C42" s="34" t="s">
+      <c r="C42" s="23" t="s">
         <v>387</v>
       </c>
-      <c r="D42" s="38" t="s">
+      <c r="D42" s="27" t="s">
         <v>230</v>
       </c>
-      <c r="E42" s="35" t="s">
+      <c r="E42" s="24" t="s">
         <v>388</v>
       </c>
-      <c r="F42" s="36" t="s">
+      <c r="F42" s="25" t="s">
         <v>389</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="27"/>
-      <c r="B43" s="33" t="s">
+      <c r="A43" s="37"/>
+      <c r="B43" s="22" t="s">
         <v>390</v>
       </c>
-      <c r="C43" s="34" t="s">
+      <c r="C43" s="23" t="s">
         <v>391</v>
       </c>
-      <c r="D43" s="38" t="s">
+      <c r="D43" s="27" t="s">
         <v>230</v>
       </c>
-      <c r="E43" s="35" t="s">
+      <c r="E43" s="24" t="s">
         <v>392</v>
       </c>
-      <c r="F43" s="36" t="s">
+      <c r="F43" s="25" t="s">
         <v>393</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="28"/>
-      <c r="B44" s="33" t="s">
+      <c r="A44" s="38"/>
+      <c r="B44" s="22" t="s">
         <v>394</v>
       </c>
-      <c r="C44" s="34" t="s">
+      <c r="C44" s="23" t="s">
         <v>395</v>
       </c>
-      <c r="D44" s="38" t="s">
+      <c r="D44" s="27" t="s">
         <v>230</v>
       </c>
-      <c r="E44" s="35" t="s">
+      <c r="E44" s="24" t="s">
         <v>396</v>
       </c>
-      <c r="F44" s="36" t="s">
+      <c r="F44" s="25" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="30" t="s">
+      <c r="A45" s="36" t="s">
         <v>398</v>
       </c>
-      <c r="B45" s="33" t="s">
+      <c r="B45" s="22" t="s">
         <v>399</v>
       </c>
-      <c r="C45" s="34" t="s">
+      <c r="C45" s="23" t="s">
         <v>400</v>
       </c>
-      <c r="D45" s="37" t="s">
+      <c r="D45" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="E45" s="35" t="s">
+      <c r="E45" s="24" t="s">
         <v>401</v>
       </c>
-      <c r="F45" s="36" t="s">
+      <c r="F45" s="25" t="s">
         <v>402</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="27"/>
-      <c r="B46" s="33" t="s">
+      <c r="A46" s="37"/>
+      <c r="B46" s="22" t="s">
         <v>403</v>
       </c>
-      <c r="C46" s="34" t="s">
+      <c r="C46" s="23" t="s">
         <v>404</v>
       </c>
-      <c r="D46" s="37" t="s">
+      <c r="D46" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="E46" s="35" t="s">
+      <c r="E46" s="24" t="s">
         <v>405</v>
       </c>
-      <c r="F46" s="36" t="s">
+      <c r="F46" s="25" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="27"/>
-      <c r="B47" s="33" t="s">
+      <c r="A47" s="37"/>
+      <c r="B47" s="22" t="s">
         <v>407</v>
       </c>
-      <c r="C47" s="34" t="s">
+      <c r="C47" s="23" t="s">
         <v>408</v>
       </c>
-      <c r="D47" s="37" t="s">
+      <c r="D47" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="E47" s="35" t="s">
+      <c r="E47" s="24" t="s">
         <v>409</v>
       </c>
-      <c r="F47" s="36" t="s">
+      <c r="F47" s="25" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="27"/>
-      <c r="B48" s="33" t="s">
+      <c r="A48" s="37"/>
+      <c r="B48" s="22" t="s">
         <v>411</v>
       </c>
-      <c r="C48" s="34" t="s">
+      <c r="C48" s="23" t="s">
         <v>412</v>
       </c>
-      <c r="D48" s="38" t="s">
+      <c r="D48" s="27" t="s">
         <v>230</v>
       </c>
-      <c r="E48" s="35" t="s">
+      <c r="E48" s="24" t="s">
         <v>413</v>
       </c>
-      <c r="F48" s="36" t="s">
+      <c r="F48" s="25" t="s">
         <v>414</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="27"/>
-      <c r="B49" s="33" t="s">
+      <c r="A49" s="37"/>
+      <c r="B49" s="22" t="s">
         <v>415</v>
       </c>
-      <c r="C49" s="34" t="s">
+      <c r="C49" s="23" t="s">
         <v>416</v>
       </c>
-      <c r="D49" s="37" t="s">
+      <c r="D49" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="E49" s="35" t="s">
+      <c r="E49" s="24" t="s">
         <v>417</v>
       </c>
-      <c r="F49" s="36" t="s">
+      <c r="F49" s="25" t="s">
         <v>418</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="27"/>
-      <c r="B50" s="33" t="s">
+      <c r="A50" s="37"/>
+      <c r="B50" s="22" t="s">
         <v>419</v>
       </c>
-      <c r="C50" s="34" t="s">
+      <c r="C50" s="23" t="s">
         <v>420</v>
       </c>
-      <c r="D50" s="37" t="s">
+      <c r="D50" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="E50" s="35" t="s">
+      <c r="E50" s="24" t="s">
         <v>421</v>
       </c>
-      <c r="F50" s="36" t="s">
+      <c r="F50" s="25" t="s">
         <v>422</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="27"/>
-      <c r="B51" s="33" t="s">
+      <c r="A51" s="37"/>
+      <c r="B51" s="22" t="s">
         <v>423</v>
       </c>
-      <c r="C51" s="34" t="s">
+      <c r="C51" s="23" t="s">
         <v>424</v>
       </c>
-      <c r="D51" s="37" t="s">
+      <c r="D51" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="E51" s="35" t="s">
+      <c r="E51" s="24" t="s">
         <v>425</v>
       </c>
-      <c r="F51" s="36" t="s">
+      <c r="F51" s="25" t="s">
         <v>426</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="28"/>
-      <c r="B52" s="33" t="s">
+      <c r="A52" s="38"/>
+      <c r="B52" s="22" t="s">
         <v>427</v>
       </c>
-      <c r="C52" s="34" t="s">
+      <c r="C52" s="23" t="s">
         <v>428</v>
       </c>
-      <c r="D52" s="37" t="s">
+      <c r="D52" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="E52" s="35" t="s">
+      <c r="E52" s="24" t="s">
         <v>429</v>
       </c>
-      <c r="F52" s="36" t="s">
+      <c r="F52" s="25" t="s">
         <v>430</v>
       </c>
     </row>
@@ -4807,76 +4897,71 @@
       <c r="D54" s="5"/>
     </row>
     <row r="55" spans="1:6" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="25" t="s">
+      <c r="A55" s="39" t="s">
         <v>431</v>
       </c>
-      <c r="B55" s="26"/>
-      <c r="C55" s="26"/>
-      <c r="D55" s="26"/>
+      <c r="B55" s="40"/>
+      <c r="C55" s="40"/>
+      <c r="D55" s="40"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="23" t="s">
+      <c r="A56" s="19" t="s">
         <v>432</v>
       </c>
-      <c r="B56" s="32" t="s">
+      <c r="B56" s="21" t="s">
         <v>433</v>
       </c>
-      <c r="C56" s="24" t="s">
+      <c r="C56" s="20" t="s">
         <v>434</v>
       </c>
-      <c r="D56" s="23" t="s">
+      <c r="D56" s="19" t="s">
         <v>435</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="41" t="s">
+      <c r="A57" s="29" t="s">
         <v>154</v>
       </c>
-      <c r="B57" s="42" t="s">
+      <c r="B57" s="30" t="s">
         <v>436</v>
       </c>
-      <c r="C57" s="43" t="s">
+      <c r="C57" s="31" t="s">
         <v>437</v>
       </c>
-      <c r="D57" s="44" t="s">
+      <c r="D57" s="32" t="s">
         <v>438</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="45" t="s">
+      <c r="A58" s="33" t="s">
         <v>156</v>
       </c>
-      <c r="B58" s="42" t="s">
+      <c r="B58" s="30" t="s">
         <v>439</v>
       </c>
-      <c r="C58" s="43" t="s">
+      <c r="C58" s="31" t="s">
         <v>440</v>
       </c>
-      <c r="D58" s="44" t="s">
+      <c r="D58" s="32" t="s">
         <v>441</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="45" t="s">
+      <c r="A59" s="33" t="s">
         <v>158</v>
       </c>
-      <c r="B59" s="42" t="s">
+      <c r="B59" s="30" t="s">
         <v>442</v>
       </c>
-      <c r="C59" s="43" t="s">
+      <c r="C59" s="31" t="s">
         <v>443</v>
       </c>
-      <c r="D59" s="44" t="s">
+      <c r="D59" s="32" t="s">
         <v>444</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="A33:A38"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A52"/>
     <mergeCell ref="A55:D55"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A3:A7"/>
@@ -4884,6 +4969,11 @@
     <mergeCell ref="A11:A17"/>
     <mergeCell ref="A18:A21"/>
     <mergeCell ref="A22:A28"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A33:A38"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>